<commit_message>
Finished all data for report 3 for RB Trees. I ran each situation 10 times and then averaged the result
</commit_message>
<xml_diff>
--- a/project3_skeleton/report3data.xlsx
+++ b/project3_skeleton/report3data.xlsx
@@ -60,6 +60,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -143,13 +144,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
-    <tabColor rgb="00FFFFFF"/>
+    <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I8" activeCellId="0" sqref="I8"/>
+      <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -213,7 +214,7 @@
         <v>0.001</v>
       </c>
       <c r="I2" s="0" t="n">
-        <v>10.35</v>
+        <v>11.73</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -238,6 +239,9 @@
       <c r="G3" s="1" t="n">
         <v>0.002</v>
       </c>
+      <c r="I3" s="0" t="n">
+        <v>11.85</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
@@ -261,6 +265,9 @@
       <c r="G4" s="1" t="n">
         <v>0.005</v>
       </c>
+      <c r="I4" s="0" t="n">
+        <v>12.71</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
@@ -284,6 +291,9 @@
       <c r="G5" s="1" t="n">
         <v>0.01</v>
       </c>
+      <c r="I5" s="0" t="n">
+        <v>11.88</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
@@ -307,6 +317,9 @@
       <c r="G6" s="1" t="n">
         <v>0.02</v>
       </c>
+      <c r="I6" s="0" t="n">
+        <v>12.65</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
@@ -329,6 +342,9 @@
       </c>
       <c r="G7" s="1" t="n">
         <v>0.04</v>
+      </c>
+      <c r="I7" s="0" t="n">
+        <v>12.26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Completed getting table 3 data (except for intersecting point)
</commit_message>
<xml_diff>
--- a/project3_skeleton/report3data.xlsx
+++ b/project3_skeleton/report3data.xlsx
@@ -149,8 +149,8 @@
   </sheetPr>
   <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H7" activeCellId="0" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -213,6 +213,9 @@
       <c r="G2" s="1" t="n">
         <v>0.001</v>
       </c>
+      <c r="H2" s="0" t="n">
+        <v>139.369</v>
+      </c>
       <c r="I2" s="0" t="n">
         <v>11.73</v>
       </c>
@@ -239,6 +242,9 @@
       <c r="G3" s="1" t="n">
         <v>0.002</v>
       </c>
+      <c r="H3" s="0" t="n">
+        <v>246.31</v>
+      </c>
       <c r="I3" s="0" t="n">
         <v>11.85</v>
       </c>
@@ -265,6 +271,9 @@
       <c r="G4" s="1" t="n">
         <v>0.005</v>
       </c>
+      <c r="H4" s="0" t="n">
+        <v>553.84</v>
+      </c>
       <c r="I4" s="0" t="n">
         <v>12.71</v>
       </c>
@@ -291,6 +300,9 @@
       <c r="G5" s="1" t="n">
         <v>0.01</v>
       </c>
+      <c r="H5" s="0" t="n">
+        <v>1028.31</v>
+      </c>
       <c r="I5" s="0" t="n">
         <v>11.88</v>
       </c>
@@ -317,6 +329,9 @@
       <c r="G6" s="1" t="n">
         <v>0.02</v>
       </c>
+      <c r="H6" s="0" t="n">
+        <v>1977.6</v>
+      </c>
       <c r="I6" s="0" t="n">
         <v>12.65</v>
       </c>
@@ -342,6 +357,9 @@
       </c>
       <c r="G7" s="1" t="n">
         <v>0.04</v>
+      </c>
+      <c r="H7" s="0" t="n">
+        <v>3666.89</v>
       </c>
       <c r="I7" s="0" t="n">
         <v>12.26</v>

</xml_diff>

<commit_message>
Completely finished report3 data. All tables are done
</commit_message>
<xml_diff>
--- a/project3_skeleton/report3data.xlsx
+++ b/project3_skeleton/report3data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="298" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="234" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="10">
   <si>
     <t>Size</t>
   </si>
@@ -51,9 +51,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="1">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
-    <numFmt numFmtId="165" formatCode="0.00%"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -120,12 +119,8 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -147,10 +142,10 @@
     <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:I8"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H7" activeCellId="0" sqref="H7"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I3" activeCellId="0" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -195,173 +190,202 @@
       <c r="A2" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="1" t="n">
-        <v>0.33</v>
-      </c>
-      <c r="C2" s="1" t="n">
-        <v>0.33</v>
-      </c>
-      <c r="D2" s="1" t="n">
-        <v>0.337</v>
-      </c>
-      <c r="E2" s="1" t="n">
-        <v>0.001</v>
-      </c>
-      <c r="F2" s="1" t="n">
-        <v>0.001</v>
-      </c>
-      <c r="G2" s="1" t="n">
-        <v>0.001</v>
+      <c r="B2" s="0" t="n">
+        <v>33</v>
+      </c>
+      <c r="C2" s="0" t="n">
+        <v>33</v>
+      </c>
+      <c r="D2" s="0" t="n">
+        <v>33.985</v>
+      </c>
+      <c r="E2" s="0" t="n">
+        <v>0.005</v>
+      </c>
+      <c r="F2" s="0" t="n">
+        <v>0.005</v>
+      </c>
+      <c r="G2" s="0" t="n">
+        <v>0.005</v>
       </c>
       <c r="H2" s="0" t="n">
-        <v>139.369</v>
+        <v>13.18</v>
       </c>
       <c r="I2" s="0" t="n">
-        <v>11.73</v>
+        <v>15.17</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="1" t="n">
-        <v>0.33</v>
-      </c>
-      <c r="C3" s="1" t="n">
-        <v>0.33</v>
-      </c>
-      <c r="D3" s="1" t="n">
-        <v>0.333</v>
-      </c>
-      <c r="E3" s="1" t="n">
-        <v>0.002</v>
-      </c>
-      <c r="F3" s="1" t="n">
-        <v>0.002</v>
-      </c>
-      <c r="G3" s="1" t="n">
-        <v>0.002</v>
+      <c r="B3" s="0" t="n">
+        <v>33</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <v>33</v>
+      </c>
+      <c r="D3" s="0" t="n">
+        <v>33.7</v>
+      </c>
+      <c r="E3" s="0" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F3" s="0" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="G3" s="0" t="n">
+        <v>0.1</v>
       </c>
       <c r="H3" s="0" t="n">
-        <v>246.31</v>
+        <v>139.369</v>
       </c>
       <c r="I3" s="0" t="n">
-        <v>11.85</v>
+        <v>11.73</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="1" t="n">
-        <v>0.33</v>
-      </c>
-      <c r="C4" s="1" t="n">
-        <v>0.33</v>
-      </c>
-      <c r="D4" s="1" t="n">
-        <v>0.325</v>
-      </c>
-      <c r="E4" s="1" t="n">
-        <v>0.005</v>
-      </c>
-      <c r="F4" s="1" t="n">
-        <v>0.005</v>
-      </c>
-      <c r="G4" s="1" t="n">
-        <v>0.005</v>
+      <c r="B4" s="0" t="n">
+        <v>33</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>33</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <v>33.4</v>
+      </c>
+      <c r="E4" s="0" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="F4" s="0" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="G4" s="0" t="n">
+        <v>0.2</v>
       </c>
       <c r="H4" s="0" t="n">
-        <v>553.84</v>
+        <v>246.31</v>
       </c>
       <c r="I4" s="0" t="n">
-        <v>12.71</v>
+        <v>11.85</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="1" t="n">
-        <v>0.32</v>
-      </c>
-      <c r="C5" s="1" t="n">
-        <v>0.32</v>
-      </c>
-      <c r="D5" s="1" t="n">
-        <v>0.33</v>
-      </c>
-      <c r="E5" s="1" t="n">
-        <v>0.01</v>
-      </c>
-      <c r="F5" s="1" t="n">
-        <v>0.01</v>
-      </c>
-      <c r="G5" s="1" t="n">
-        <v>0.01</v>
+      <c r="B5" s="0" t="n">
+        <v>33</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>33</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>32.5</v>
+      </c>
+      <c r="E5" s="0" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="F5" s="0" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="G5" s="0" t="n">
+        <v>0.5</v>
       </c>
       <c r="H5" s="0" t="n">
-        <v>1028.31</v>
+        <v>553.84</v>
       </c>
       <c r="I5" s="0" t="n">
-        <v>11.88</v>
+        <v>12.71</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="1" t="n">
-        <v>0.31</v>
-      </c>
-      <c r="C6" s="1" t="n">
-        <v>0.31</v>
-      </c>
-      <c r="D6" s="1" t="n">
-        <v>0.32</v>
-      </c>
-      <c r="E6" s="1" t="n">
-        <v>0.02</v>
-      </c>
-      <c r="F6" s="1" t="n">
-        <v>0.02</v>
-      </c>
-      <c r="G6" s="1" t="n">
-        <v>0.02</v>
+      <c r="B6" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="C6" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="D6" s="0" t="n">
+        <v>33</v>
+      </c>
+      <c r="E6" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F6" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G6" s="0" t="n">
+        <v>1</v>
       </c>
       <c r="H6" s="0" t="n">
-        <v>1977.6</v>
+        <v>1028.31</v>
       </c>
       <c r="I6" s="0" t="n">
-        <v>12.65</v>
+        <v>11.88</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="1" t="n">
-        <v>0.29</v>
-      </c>
-      <c r="C7" s="1" t="n">
-        <v>0.29</v>
-      </c>
-      <c r="D7" s="1" t="n">
-        <v>0.3</v>
-      </c>
-      <c r="E7" s="1" t="n">
-        <v>0.04</v>
-      </c>
-      <c r="F7" s="1" t="n">
-        <v>0.04</v>
-      </c>
-      <c r="G7" s="1" t="n">
-        <v>0.04</v>
+      <c r="B7" s="0" t="n">
+        <v>31</v>
+      </c>
+      <c r="C7" s="0" t="n">
+        <v>31</v>
+      </c>
+      <c r="D7" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="E7" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F7" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="G7" s="0" t="n">
+        <v>2</v>
       </c>
       <c r="H7" s="0" t="n">
+        <v>1977.6</v>
+      </c>
+      <c r="I7" s="0" t="n">
+        <v>12.65</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="0" t="n">
+        <v>29</v>
+      </c>
+      <c r="C8" s="0" t="n">
+        <v>29</v>
+      </c>
+      <c r="D8" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="E8" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="F8" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="G8" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="H8" s="0" t="n">
         <v>3666.89</v>
       </c>
-      <c r="I7" s="0" t="n">
+      <c r="I8" s="0" t="n">
         <v>12.26</v>
       </c>
     </row>

</xml_diff>